<commit_message>
modify script & data sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Weldon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivian/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1D31D3-6E95-4291-A751-AE7C99CB3662}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F750B4BA-CA0B-0D45-8597-78174B9A8D37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{63BF1483-597D-48B4-8626-BE0D0A5D7BAB}"/>
+    <workbookView xWindow="7480" yWindow="1580" windowWidth="23040" windowHeight="9080" xr2:uid="{63BF1483-597D-48B4-8626-BE0D0A5D7BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Almond milk</t>
   </si>
@@ -186,13 +181,151 @@
   </si>
   <si>
     <t>Global Warming Potential (GWP)</t>
+  </si>
+  <si>
+    <t>Images URL</t>
+  </si>
+  <si>
+    <t>https://nutriliving-images.imgix.net/images/2014/336/12909/A08F59E7-567A-E411-A121-0287E8A1303A.jpg?ch=DPR&amp;w=500&amp;h=500&amp;auto=compress,format&amp;dpr=1&amp;ixlib=imgixjs-3.0.4</t>
+  </si>
+  <si>
+    <t>https://www.organicfacts.net/wp-content/uploads/almondsnutrition.jpg</t>
+  </si>
+  <si>
+    <t>http://onedaycart.com/media/catalog/product/cache/1/image/9df78eab33525d08d6e5fb8d27136e95/b/e/beef_3.jpg</t>
+  </si>
+  <si>
+    <t>https://hummersmeats.com/wp-content/uploads/IMG_0153.jpg</t>
+  </si>
+  <si>
+    <t>http://www.whitehall-specialties.com/wp-content/uploads/2014/01/sos-iws.jpg</t>
+  </si>
+  <si>
+    <t>https://3ner1e34iilsjdn1qohanunu-wpengine.netdna-ssl.com/wp-content/uploads/2015/05/shutterstock-SherryCheeseSpread-540x360.jpg</t>
+  </si>
+  <si>
+    <t>https://schrammsflowers.com/wp-content/uploads/2017/12/chocolate-600x600.jpg</t>
+  </si>
+  <si>
+    <t>https://www.thespruceeats.com/thmb/nnQ-XscEfo2P8hjNkfoxFqglvAg=/960x0/filters:no_upscale():max_bytes(150000):strip_icc():format(webp)/chocolate-milk-489225125-5ac400223418c600376611f0.jpg</t>
+  </si>
+  <si>
+    <t>https://www.naturalfoodseries.com/wp-content/uploads/2017/10/Corn.jpg</t>
+  </si>
+  <si>
+    <t>http://organicityproject.eu/images/Fotolia_64976600_XS.jpg</t>
+  </si>
+  <si>
+    <t>http://www.josephsgourmetpasta.com/wp-content/uploads/2014/09/BRAISED-BEEF-High-Res-1000x400.png</t>
+  </si>
+  <si>
+    <t>https://www.park4pizza.com.au/wp-content/uploads/2017/09/IMG_0603-600x400.jpg</t>
+  </si>
+  <si>
+    <t>https://www.coopathome.ch/img/produkte/300_300/RGB/3362114_002.jpg?_=1474362648643</t>
+  </si>
+  <si>
+    <t>https://divinefishandmeat.com/wp-content/uploads/sfr-boneless-ham-cooked-web_1.jpg</t>
+  </si>
+  <si>
+    <t>https://atmedia.imgix.net/3bb3810e845c333ff6d117448f4bdc95b551d8ce?auto=format&amp;q=45&amp;w=1033.0&amp;fit=max&amp;cs=strip</t>
+  </si>
+  <si>
+    <t>https://www.humboldtcreamery.com/wp-content/uploads/2017/08/Organic-Low-Fat-Milk.png</t>
+  </si>
+  <si>
+    <t>https://sfbay.cropmobster.com/wp-content/uploads/sites/2/IMG_79362-900x500.jpg</t>
+  </si>
+  <si>
+    <t>https://www.bellavitashop.co.uk/1622-large_default/pancetta-di-piacenza-.jpg</t>
+  </si>
+  <si>
+    <t>https://theglamorousgourmet.com/wp-content/uploads/2014/08/PROVENCAL-PORK-CHOPS-RAW.jpg</t>
+  </si>
+  <si>
+    <t>https://www.trunkey.com.au/wp-content/uploads/2017/09/601-602-607-Fresh-Gourmet-Sausages.jpg</t>
+  </si>
+  <si>
+    <t>http://3.bp.blogspot.com/-CaPgx6K2k6U/VkJwW5JrSeI/AAAAAAAAKBQ/2ATdx0nGotM/s1600/20151110-vegan-chicken-pieces-quorn-meat-free-1-packs.jpg</t>
+  </si>
+  <si>
+    <t>https://5.imimg.com/data5/JX/AB/MY-14534935/red-kidney-beans-500x500.jpg</t>
+  </si>
+  <si>
+    <t>https://www.organicfacts.net/wp-content/uploads/ricemilk-700x525.jpg</t>
+  </si>
+  <si>
+    <t>http://www.bite.co.nz/images/recipes/Generic_Rice_Risotto1.jpg?width=1200&amp;height=800</t>
+  </si>
+  <si>
+    <t>https://s3.amazonaws.com/jconline/470_250_usugiri.jpg</t>
+  </si>
+  <si>
+    <t>https://www.fifteenspatulas.com/wp-content/uploads/2012/10/ThinSlicedChicken__FifteenSpatulas.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dutchcheeses.com/wp-content/uploads/2015/05/rook_kaas_21427988883551d61938fd86.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/productImages/550/55025011_0_640x640.jpg?identifier=6a4d4b34e166c88409794184413675dc</t>
+  </si>
+  <si>
+    <t>https://atmedia.imgix.net/249f12fcc476b9cce640f6d3689efa89be8ac615?auto=format&amp;q=45&amp;w=600.0&amp;h=750.0&amp;fit=max&amp;cs=strip</t>
+  </si>
+  <si>
+    <t>http://eurofit.be/wp-content/uploads/2014/03/Thumb_semi-skimmed-milk.jpg</t>
+  </si>
+  <si>
+    <t>http://yvesveggie.com/media/1972/veggie-salami_clean-ingredient_consept_us.png</t>
+  </si>
+  <si>
+    <t>http://www.foodsaver.com.cy/udata/contents/images/Products/Dry%20food_Sauces/Pastas/tn/pomais_penne_uncooked7_400_800_crp.jpg</t>
+  </si>
+  <si>
+    <t>https://images.anovaculinary.com/sous-vide-rack-of-lamb/directions/sous-vide-rack-of-lamb-directions-image-1.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn1.medicalnewstoday.com/content/images/articles/321/321990/close-up-of-block-of-butter-being-sliced-may-raise-cholesterol.jpg</t>
+  </si>
+  <si>
+    <t>https://4.imimg.com/data4/VQ/UC/MY-21617981/turkey-chicken-500x500.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/30/RabbitMilwaukee.jpg/1200px-RabbitMilwaukee.jpg</t>
+  </si>
+  <si>
+    <t>https://secure.i.telegraph.co.uk/multimedia/archive/02884/cod_2884916b.jpg</t>
+  </si>
+  <si>
+    <t>https://i.kinja-img.com/gawker-media/image/upload/s--m6hjGHRf--/c_scale,f_auto,fl_progressive,q_80,w_800/aapfqrjiromx7x1m6rgy.jpg</t>
+  </si>
+  <si>
+    <t>https://i1.wp.com/lenews.ch/wp-content/uploads/2016/12/Insect-street-food-China_%C2%A9-Anastasiia-Maltseva-Dreamstime.com_.jpg?w=800&amp;ssl=1</t>
+  </si>
+  <si>
+    <t>https://groceries.iceland.co.uk/medias/sys_master/root/h08/h78/8844344557598.jpg</t>
+  </si>
+  <si>
+    <t>https://sc02.alicdn.com/kf/UT8dtVlXJNXXXagOFbX0/WHEAT.jpg_350x350.jpg</t>
+  </si>
+  <si>
+    <t>https://www.almanac.com/sites/default/files/styles/primary_image_in_article/public/image_nodes/peas-and-pea-pods.jpg?itok=J2VmdFCz</t>
+  </si>
+  <si>
+    <t>https://3ztzui4amtxs1wdjlrh1061b-wpengine.netdna-ssl.com/wp-content/uploads/4.11_MOT_Barley_NEW-Wordpress.gif</t>
+  </si>
+  <si>
+    <t>https://cdn1.medicalnewstoday.com/content/images/articles/280/280244/chickpeas-in-a-bowl.jpg</t>
+  </si>
+  <si>
+    <t>https://5.imimg.com/data5/CO/BO/MY-47677163/live-white-chicken--500x500.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +354,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -236,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -259,13 +400,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -280,8 +433,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4CE7E80E-49AC-4417-8CC8-41ABF6B79854}"/>
     <cellStyle name="Normal 4" xfId="2" xr:uid="{22CA73B9-4CC7-4A4F-BE8F-538342351AFE}"/>
@@ -596,21 +752,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6992AFDA-6D9F-465C-907C-B64B9B421592}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="6" t="s">
         <v>50</v>
@@ -622,7 +778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>45</v>
@@ -633,8 +789,11 @@
       <c r="D2" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,8 +806,11 @@
       <c r="D3" s="7">
         <v>1.0898783206332101</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,8 +823,11 @@
       <c r="D4" s="7">
         <v>1.9013045715911601</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -675,8 +840,11 @@
       <c r="D5" s="7">
         <v>0.469425987022143</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -689,8 +857,11 @@
       <c r="D6" s="7">
         <v>0.14570166801345499</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -703,8 +874,11 @@
       <c r="D7" s="7">
         <v>0.108737614894822</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -717,8 +891,11 @@
       <c r="D8" s="7">
         <v>0.33902140273791398</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -731,8 +908,11 @@
       <c r="D9" s="7">
         <v>0.37513623312745797</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -745,8 +925,11 @@
       <c r="D10" s="7">
         <v>0.11053844368761952</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -759,8 +942,11 @@
       <c r="D11" s="7">
         <v>5.725737294377E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -773,8 +959,11 @@
       <c r="D12" s="7">
         <v>0.469425987022143</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -787,8 +976,11 @@
       <c r="D13" s="7">
         <v>1.18891713900774E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -801,8 +993,11 @@
       <c r="D14" s="7">
         <v>0.16438500312310583</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -815,8 +1010,11 @@
       <c r="D15" s="7">
         <v>4.4167568693069773E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -829,8 +1027,11 @@
       <c r="D16" s="7">
         <v>0.14570166801345499</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -843,8 +1044,11 @@
       <c r="D17" s="7">
         <v>0.52107065489710402</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -857,8 +1061,11 @@
       <c r="D18" s="7">
         <v>0.13569536742406299</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -871,8 +1078,11 @@
       <c r="D19" s="7">
         <v>1.4149503710495399E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -885,8 +1095,11 @@
       <c r="D20" s="7">
         <v>0.18456657454426301</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -899,8 +1112,11 @@
       <c r="D21" s="7">
         <v>0.52107065489710402</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -913,8 +1129,11 @@
       <c r="D22" s="7">
         <v>0.52107065489710402</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -927,8 +1146,11 @@
       <c r="D23" s="7">
         <v>0.52107065489710402</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -941,8 +1163,11 @@
       <c r="D24" s="7">
         <v>5.725737294377E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -955,8 +1180,11 @@
       <c r="D25" s="7">
         <v>0.13569536742406299</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -969,8 +1197,11 @@
       <c r="D26" s="7">
         <v>0.25712987138015753</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -983,8 +1214,11 @@
       <c r="D27" s="7">
         <v>0.35153526300458998</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -997,8 +1231,11 @@
       <c r="D28" s="7">
         <v>0.469425987022143</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1011,8 +1248,11 @@
       <c r="D29" s="4">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1025,8 +1265,11 @@
       <c r="D30" s="7">
         <v>0.108737614894822</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1039,8 +1282,11 @@
       <c r="D31" s="7">
         <v>0.10953513289494721</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1053,8 +1299,11 @@
       <c r="D32" s="7">
         <v>4.2499828861568096E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -1067,8 +1316,11 @@
       <c r="D33" s="7">
         <v>2.2339180541006701E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1081,8 +1333,11 @@
       <c r="D34" s="7">
         <v>5.725737294377E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -1095,8 +1350,11 @@
       <c r="D35" s="7">
         <v>1.18891713900774E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1105,8 +1363,11 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -1115,8 +1376,11 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -1125,8 +1389,11 @@
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1135,8 +1402,11 @@
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -1145,8 +1415,11 @@
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -1155,8 +1428,11 @@
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -1165,8 +1441,11 @@
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
@@ -1175,8 +1454,11 @@
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1185,8 +1467,11 @@
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -1195,8 +1480,11 @@
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -1205,8 +1493,11 @@
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>6</v>
       </c>
@@ -1215,9 +1506,45 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
+      <c r="E47" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1" xr:uid="{637889EC-A1B4-8048-95E6-E95BE28AD54D}"/>
+    <hyperlink ref="E17" r:id="rId2" xr:uid="{F9A98115-C22F-9346-BAD9-700CC638D641}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{FAAAFB40-8348-BB4C-A7A9-547D9D9D8A3D}"/>
+    <hyperlink ref="E19" r:id="rId4" xr:uid="{96CA0D9D-8CA3-4D41-B59B-51F1A6693EEE}"/>
+    <hyperlink ref="E20" r:id="rId5" xr:uid="{AE924BC2-08C5-194A-BD69-C15E08278729}"/>
+    <hyperlink ref="E21" r:id="rId6" xr:uid="{46F7C017-DA52-7B4C-99B0-77C942A25AD8}"/>
+    <hyperlink ref="E22" r:id="rId7" xr:uid="{D5C2177F-A067-654A-BE0E-47E33D4D80E8}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{513A2576-89F6-1944-8D0C-3CDCC17112A4}"/>
+    <hyperlink ref="E24" r:id="rId9" xr:uid="{7ECDF753-B816-584D-91EF-2A2221D1EDE0}"/>
+    <hyperlink ref="E25" r:id="rId10" xr:uid="{F8B1E67B-7426-E646-A284-3782B4ED310C}"/>
+    <hyperlink ref="E26" r:id="rId11" xr:uid="{9BD2EA01-CDE8-644A-9C2D-6B9CAC0657CB}"/>
+    <hyperlink ref="E27" r:id="rId12" xr:uid="{81560DB9-5ABB-0844-B276-7334C818AADD}"/>
+    <hyperlink ref="E28" r:id="rId13" xr:uid="{491581CB-5A43-E542-8924-CEA62E4E30F4}"/>
+    <hyperlink ref="E30" r:id="rId14" xr:uid="{BA8D4B11-6493-8949-B78F-8C7EB7A57C4E}"/>
+    <hyperlink ref="E31" r:id="rId15" xr:uid="{6C050EE2-23F7-F34B-8EF2-A0E77FB321AF}"/>
+    <hyperlink ref="E32" r:id="rId16" xr:uid="{B22F2DF1-15F8-6140-A578-A2C5AD430D31}"/>
+    <hyperlink ref="E33" r:id="rId17" xr:uid="{6C15C962-CD7B-794F-B547-E23D3D42E869}"/>
+    <hyperlink ref="E34" r:id="rId18" xr:uid="{3DFCD2FD-4E77-EB48-A7B2-12D59859FC39}"/>
+    <hyperlink ref="E35" r:id="rId19" xr:uid="{2D3B00D1-6C12-4D49-8E51-97D4363BAEF3}"/>
+    <hyperlink ref="E36" r:id="rId20" xr:uid="{7B977F22-5C88-824E-AA5D-A629CE7665E2}"/>
+    <hyperlink ref="E37" r:id="rId21" xr:uid="{A5F840C4-4A6E-C648-85DF-6107E436C5A5}"/>
+    <hyperlink ref="E38" r:id="rId22" xr:uid="{2591EA3E-33AD-C44A-B481-DCCAABE0FB7C}"/>
+    <hyperlink ref="E39" r:id="rId23" xr:uid="{3E5ACC63-D902-5046-BC96-929FD8631066}"/>
+    <hyperlink ref="E40" r:id="rId24" xr:uid="{A4A72284-9257-814A-9846-967E35DC0966}"/>
+    <hyperlink ref="E41" r:id="rId25" xr:uid="{69F6F143-454B-EE41-8A61-053679CA0C71}"/>
+    <hyperlink ref="E42" r:id="rId26" xr:uid="{CAFA2FF4-0523-FA4E-B067-BB01E7BD6463}"/>
+    <hyperlink ref="E43" r:id="rId27" xr:uid="{A24C0B89-3540-C442-A30D-4C355F1E9FE0}"/>
+    <hyperlink ref="E44" r:id="rId28" xr:uid="{FCA666E9-C7D5-4249-9856-8A7D2FB12F15}"/>
+    <hyperlink ref="E45" r:id="rId29" xr:uid="{697A448A-5384-8144-A909-84C14F9C527B}"/>
+    <hyperlink ref="E46" r:id="rId30" xr:uid="{2F6E2CA5-E9A1-644B-82B3-568289D72E6A}"/>
+    <hyperlink ref="E47" r:id="rId31" xr:uid="{8005F884-C04F-B349-B5A4-31CD27EA653B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>